<commit_message>
Display dates, Color, and width of columns
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002273D1"/>
+        <bgColor rgb="002273D1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,38 +427,45 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, July 18, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, July 19, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, July 20, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, July 21, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, July 22, 2023</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arrival Time</t>
+          <t>Arrival</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,7 +485,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Arrival Time</t>
+          <t>Arrival</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -491,7 +505,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Arrival Time</t>
+          <t>Arrival</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -511,7 +525,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Arrival Time</t>
+          <t>Arrival</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -531,7 +545,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Arrival Time</t>
+          <t>Arrival</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">

</xml_diff>